<commit_message>
nice ... hoffentlich klappt das jetzt noch Oo
</commit_message>
<xml_diff>
--- a/Bricks/Bibelvers/Bibelverse.xlsx
+++ b/Bricks/Bibelvers/Bibelverse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dyrian\github\Aaron\Bricks\Bibelvers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DD7395-0384-4963-ABC8-5AE40275457B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538017C9-E3AA-4C4B-8166-3D46E8E0B4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Bibelverse</t>
   </si>
@@ -90,7 +90,52 @@
     <t>"Ich habe dich je und je geliebt, darum habe ich dich zu mir gezogen, aus lauter Güte." (Jeremia 31, 3)</t>
   </si>
   <si>
-    <t>"Wir sehen jetzt durch einen Spiegel ein dunkles Bild; dann aber von Angesicht zu Angesicht. Jetzt erkenne ich stückweise; dann aber werde ich erkennen, wie ich erkannt bin. Nun aber bleiben Glaube, Hoffnung, Liebe, diese drei; aber die Liebe ist die größte unter ihnen." (1Korinther 13,12+13)</t>
+    <t>"Denn wir sehen jetzt durch einen Spiegel ein undeutliches Bild, dann aber, sehen wir von Angesicht zu Angesicht. Jetzt erkenne ich stückweise, dann aber werde ich erkennen, wie auch ich erkannt worden bin."  (1. Korinther 13,12)</t>
+  </si>
+  <si>
+    <t>Bibelstelle</t>
+  </si>
+  <si>
+    <t>1 Kor 13,12</t>
+  </si>
+  <si>
+    <t>Joh 16,22</t>
+  </si>
+  <si>
+    <t>2 Tim 1,10</t>
+  </si>
+  <si>
+    <t>1 Kor 15,27</t>
+  </si>
+  <si>
+    <t>Jer 31,3</t>
+  </si>
+  <si>
+    <t>Joh 10,27f.</t>
+  </si>
+  <si>
+    <t>Ps 118,6</t>
+  </si>
+  <si>
+    <t>Ps 145,14</t>
+  </si>
+  <si>
+    <t>Jes 43,1b</t>
+  </si>
+  <si>
+    <t>Jes 54,10</t>
+  </si>
+  <si>
+    <t>2 Kor 5,1</t>
+  </si>
+  <si>
+    <t>1 Mos 24,56</t>
+  </si>
+  <si>
+    <t>Ps 37,5</t>
+  </si>
+  <si>
+    <t>5 Mos 4,31</t>
   </si>
 </sst>
 </file>
@@ -427,146 +472,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C18"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="177.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ansprache wird jetzt unterstützt Todo: Formatierung Dokument und Ansprache: Hand und Säule ...
</commit_message>
<xml_diff>
--- a/Bricks/Bibelvers/Bibelverse.xlsx
+++ b/Bricks/Bibelvers/Bibelverse.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dyrian\github\Aaron\Bricks\Bibelvers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Dörr\PycharmProjects\Aaron\Bricks\Bibelvers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538017C9-E3AA-4C4B-8166-3D46E8E0B4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51F3819-2A86-4533-8E8D-E8723539AC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Bibelverse</t>
   </si>
@@ -39,21 +50,12 @@
     <t>"Halte mich nicht auf, denn der Herr hat Gnade zu meiner Reise gegeben. Lasset mich, dass ich zu meinem Herrn ziehe." (1.Mose 24, 56)</t>
   </si>
   <si>
-    <t>Weg</t>
-  </si>
-  <si>
     <t>"Befiehl dem Herrn deine Wege und hoffe auf ihn, er wird's wohl machen." (Psalm 37, 5 )</t>
   </si>
   <si>
     <t>"Ihr seid jetzt traurig, aber ich werde euch wiedersehen. Dann wird euer Herz sich freuen, und eure Freude wird euch niemand nehmen." (Johannes 16, 22)</t>
   </si>
   <si>
-    <t>Freude</t>
-  </si>
-  <si>
-    <t>Psalm23</t>
-  </si>
-  <si>
     <t>"Meine Schafe hören meine Stimme und ich kenne sie, und ich gebe ihnen das ewige Leben, und niemand wird sie aus meiner Hand reißen." (Johannes 10,27f.)</t>
   </si>
   <si>
@@ -72,15 +74,9 @@
     <t>"Der Herr hält alle, die da fallen, und richtet alle auf, die niedergeschlagen sind." (Psalm 145,14)</t>
   </si>
   <si>
-    <t>Bild</t>
-  </si>
-  <si>
     <t>"Es mögen wohl Berge weichen und Hügel hinfallen. Aber meine Hilfe soll nicht von dir weichen." (Jesaja 54,10)</t>
   </si>
   <si>
-    <t>"Gott aber sei Dank, der uns den Sieg gegeben hat durch unseren Herrn Jesus Christus" (1. Korinther 15,57)</t>
-  </si>
-  <si>
     <t xml:space="preserve">"Der Herr, dein Gott, ist ein barmherziger Gott; er wird dich nicht verlassen" (5. Mose 4, 31) </t>
   </si>
   <si>
@@ -105,9 +101,6 @@
     <t>2 Tim 1,10</t>
   </si>
   <si>
-    <t>1 Kor 15,27</t>
-  </si>
-  <si>
     <t>Jer 31,3</t>
   </si>
   <si>
@@ -136,6 +129,36 @@
   </si>
   <si>
     <t>5 Mos 4,31</t>
+  </si>
+  <si>
+    <t>Psalm23, Weg</t>
+  </si>
+  <si>
+    <t>Bild, Regenbogen</t>
+  </si>
+  <si>
+    <t>Weg, Regenbogen, Bild</t>
+  </si>
+  <si>
+    <t>Weg, Fluss, Psalm23, Hand</t>
+  </si>
+  <si>
+    <t>Psalm23, Hand</t>
+  </si>
+  <si>
+    <t>Psalm23, Weg, Fluss</t>
+  </si>
+  <si>
+    <t>Psalm23, Hand, Säulen</t>
+  </si>
+  <si>
+    <t>Säulen, Hand</t>
+  </si>
+  <si>
+    <t>Weg, Fluss, Regenbogen</t>
+  </si>
+  <si>
+    <t>Weg, Fluss</t>
   </si>
 </sst>
 </file>
@@ -472,30 +495,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="177.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="177.44140625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -503,175 +526,164 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
-        <v>3</v>
-      </c>
       <c r="D16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:C18">
-    <sortCondition ref="B5:B18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:C17">
+    <sortCondition ref="B5:B17"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B2:C3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B27" xr:uid="{2E807EAB-3D8C-44AD-ACD7-0FF74E63E25D}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B25" xr:uid="{2E807EAB-3D8C-44AD-ACD7-0FF74E63E25D}">
       <formula1>"Weg;Freude;Psalm23;Säulen;Bild"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B14 B29 B16:B22" xr:uid="{D211DF65-9784-43F9-942B-5400574D5B85}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27" xr:uid="{D211DF65-9784-43F9-942B-5400574D5B85}">
       <formula1>"Weg,Freude,Psalm23,Säulen,Bild"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>